<commit_message>
Adding some documents from previous project directory & reorganize wiring (document) & update listOfMaterials
</commit_message>
<xml_diff>
--- a/Documentation/ListOfMaterials.xlsx
+++ b/Documentation/ListOfMaterials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Plastic Case</t>
   </si>
   <si>
-    <t>Fuses holder</t>
-  </si>
-  <si>
-    <t>Fuses 20A</t>
-  </si>
-  <si>
     <t>Current sensor (Hall)</t>
   </si>
   <si>
@@ -128,6 +122,12 @@
   </si>
   <si>
     <t>Led multicolor (Blue/Red/Green)</t>
+  </si>
+  <si>
+    <t>Current sensor (GFCI)</t>
+  </si>
+  <si>
+    <t>Digikey</t>
   </si>
 </sst>
 </file>
@@ -538,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M26"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>2</v>
@@ -573,16 +573,16 @@
         <v>3</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:13">
       <c r="B4" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -595,32 +595,32 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="7"/>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F22" si="0">E5*D5</f>
+        <f t="shared" ref="F5:F21" si="0">E5*D5</f>
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -642,16 +642,16 @@
         <v>4</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:13">
       <c r="B7" s="7"/>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -661,16 +661,16 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="7"/>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -680,16 +680,16 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="7"/>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -702,35 +702,41 @@
         <v>31</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="7"/>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>9.2899999999999991</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.579999999999998</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="7"/>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -740,295 +746,277 @@
         <v>31</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="7"/>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>9.2899999999999991</v>
+        <v>29.5</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>18.579999999999998</v>
+        <v>29.5</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="7"/>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="E13">
+        <v>10.53</v>
+      </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.53</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="7"/>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>29.5</v>
-      </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>29.5</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:13">
       <c r="B15" s="7"/>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15" s="5">
+        <v>191.55</v>
+      </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>191.55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" s="7"/>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" s="5">
-        <v>191.55</v>
+        <v>1.54</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>191.55</v>
+        <v>1.54</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="7"/>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" s="5">
-        <v>1.54</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>1.54</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="7"/>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" s="5">
-        <v>1.1599999999999999</v>
+        <v>1.67</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>1.1599999999999999</v>
+        <v>1.67</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="7"/>
-      <c r="C19" t="s">
+      <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="5">
-        <v>1.67</v>
+      <c r="E19">
+        <v>9.31</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>9.31</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20">
-        <v>9.31</v>
-      </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>9.31</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="8"/>
-      <c r="C21" s="3" t="s">
-        <v>25</v>
+      <c r="C21" t="s">
+        <v>24</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21">
+        <v>22.06</v>
+      </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.06</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="8"/>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>22.06</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>22.06</v>
-      </c>
-      <c r="G22" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="F24">
+        <f>SUM(F4:F21)</f>
+        <v>365.89000000000004</v>
       </c>
     </row>
     <row r="25" spans="2:10">
-      <c r="F25">
-        <f>SUM(F4:F22)</f>
-        <v>355.36000000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26">
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
         <v>12.47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:B19"/>
-    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B4:B18"/>
+    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J12" r:id="rId1"/>
-    <hyperlink ref="K16" r:id="rId2"/>
-    <hyperlink ref="L16" r:id="rId3"/>
-    <hyperlink ref="M16" r:id="rId4"/>
-    <hyperlink ref="J16" r:id="rId5"/>
-    <hyperlink ref="J17" r:id="rId6"/>
-    <hyperlink ref="J18" r:id="rId7"/>
-    <hyperlink ref="J19" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId1"/>
+    <hyperlink ref="K15" r:id="rId2"/>
+    <hyperlink ref="L15" r:id="rId3"/>
+    <hyperlink ref="M15" r:id="rId4"/>
+    <hyperlink ref="J15" r:id="rId5"/>
+    <hyperlink ref="J16" r:id="rId6"/>
+    <hyperlink ref="J17" r:id="rId7"/>
+    <hyperlink ref="J18" r:id="rId8"/>
+    <hyperlink ref="J13" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating list of material
</commit_message>
<xml_diff>
--- a/Documentation/ListOfMaterials.xlsx
+++ b/Documentation/ListOfMaterials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -122,13 +122,19 @@
   </si>
   <si>
     <t xml:space="preserve">Type 2 plug &amp; cord </t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Shipment fee openEVSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,8 +164,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +196,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -204,7 +222,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -212,8 +230,9 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -229,18 +248,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="2" builtinId="25"/>
@@ -535,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M24"/>
+  <dimension ref="B2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G18" sqref="G16:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -577,13 +600,13 @@
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:13">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
@@ -607,7 +630,7 @@
       </c>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -626,7 +649,7 @@
       </c>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="7"/>
+      <c r="B6" s="8"/>
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -644,8 +667,8 @@
       <c r="G6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
+      <c r="H6" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>23</v>
@@ -655,7 +678,7 @@
       </c>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="7"/>
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>17</v>
       </c>
@@ -674,7 +697,7 @@
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="7"/>
+      <c r="B8" s="8"/>
       <c r="C8" t="s">
         <v>16</v>
       </c>
@@ -693,7 +716,7 @@
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="7"/>
+      <c r="B9" s="8"/>
       <c r="C9" t="s">
         <v>15</v>
       </c>
@@ -712,7 +735,7 @@
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="7"/>
+      <c r="B10" s="8"/>
       <c r="C10" t="s">
         <v>22</v>
       </c>
@@ -737,7 +760,7 @@
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" t="s">
         <v>24</v>
       </c>
@@ -756,7 +779,7 @@
       </c>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" t="s">
         <v>32</v>
       </c>
@@ -774,8 +797,8 @@
       <c r="G12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>10</v>
+      <c r="H12" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="I12" t="s">
         <v>23</v>
@@ -785,7 +808,7 @@
       </c>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -803,8 +826,8 @@
       <c r="G13" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>10</v>
+      <c r="H13" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="I13" t="s">
         <v>23</v>
@@ -814,7 +837,7 @@
       </c>
     </row>
     <row r="14" spans="2:13">
-      <c r="B14" s="7"/>
+      <c r="B14" s="8"/>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -830,7 +853,7 @@
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="7"/>
+      <c r="B15" s="8"/>
       <c r="C15" t="s">
         <v>35</v>
       </c>
@@ -847,8 +870,8 @@
       <c r="G15" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>10</v>
+      <c r="H15" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>26</v>
@@ -864,7 +887,7 @@
       </c>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="7"/>
+      <c r="B16" s="8"/>
       <c r="C16" t="s">
         <v>18</v>
       </c>
@@ -889,7 +912,7 @@
       </c>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="7"/>
+      <c r="B17" s="8"/>
       <c r="C17" t="s">
         <v>31</v>
       </c>
@@ -914,7 +937,7 @@
       </c>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="7"/>
+      <c r="B18" s="8"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -939,7 +962,7 @@
       </c>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -966,7 +989,7 @@
       </c>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="8"/>
+      <c r="B20" s="9"/>
       <c r="C20" t="s">
         <v>21</v>
       </c>
@@ -1000,8 +1023,23 @@
       <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>12.47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25">
+        <f>26.37/1.2</f>
+        <v>21.975000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="F27">
+        <f>F23+F24+F25</f>
+        <v>417.82333333333338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>